<commit_message>
200408 Update All Files
</commit_message>
<xml_diff>
--- a/02 Scheduler/200407_hexapod_WBS.xlsx
+++ b/02 Scheduler/200407_hexapod_WBS.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Hexapod\02 Scheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E090303C-EBC2-4F3B-83F9-0B5CB7CC5135}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4465B9FC-5A50-49F0-8414-2E9C410B56F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19665" yWindow="5475" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wbs" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">wbs!$A$1:$AC$30</definedName>
@@ -1654,8 +1655,8 @@
   </sheetPr>
   <dimension ref="A1:DU40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6310,4 +6311,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="66" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8913F3BD-17AF-4F0C-94AF-37A1DB903063}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>